<commit_message>
0.0.3 - microstick now has a response curve
</commit_message>
<xml_diff>
--- a/TQS_debugging/curve_debugging.xlsx
+++ b/TQS_debugging/curve_debugging.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="14880" windowHeight="6330"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="14880" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>relativePos</t>
   </si>
@@ -50,12 +51,18 @@
   <si>
     <t>mapped</t>
   </si>
+  <si>
+    <t>f(I) = I^(3-(s/4.5))</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +70,12 @@
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,6 +712,601 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>curveFactor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-0.54545454545454541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.45454545454545453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.40909090909090912</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.31818181818181818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.27272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.22727272727272727</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.13636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.5454545454545456E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.5454545454545456E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.22727272727272727</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.27272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.31818181818181818</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-0.24309161870377496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.19842513149602492</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.15885970244393161</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.12423565864449228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.4382261884774651E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.9115561102646786E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.8235486406878095E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.152175734685652E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.8727812725378663E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.571132733059505E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.7160687026661894E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-7.3736142097480207E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3736142097480207E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7160687026661894E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.571132733059505E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8727812725378663E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.152175734685652E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8235486406878095E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9115561102646786E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.4382261884774651E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$F$2:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="166088704"/>
+        <c:axId val="166090240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="166088704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="166090240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="166090240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="166088704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mapped</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$E$2:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>70.677334127992609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.118125512804198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.366544553731003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.459914791849926</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.43814628443393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.34423759225632</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116.22495505239225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120.13178922017228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>123.12237377544274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>125.26274772364737</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>126.63136894075178</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>127.32764176784714</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>127.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>127.67235823215286</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>128.36863105924823</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>129.73725227635265</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131.87762622455728</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>134.86821077982771</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>138.77504494760774</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>143.65576240774368</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>149.56185371556609</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>156.54008520815006</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>164.63345544626901</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>173.88187448719583</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>184.32266587200741</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="166108544"/>
+        <c:axId val="165971072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="166108544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165971072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="165971072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="166108544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -744,6 +1355,75 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1052,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2527,13 +3207,1533 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <f>(A2-$J$6)/$J$6</f>
+        <v>-0.54545454545454541</v>
+      </c>
+      <c r="C2">
+        <f>IF(B2&lt;0,-1*POWER(ABS(B2),(3-($J$3/4.5))),POWER(ABS(B2),(3-($J$3/4.5))))</f>
+        <v>-0.24309161870377496</v>
+      </c>
+      <c r="D2">
+        <f>($J$6*C2)+$J$6</f>
+        <v>416.29960971292377</v>
+      </c>
+      <c r="E2">
+        <f>IF(D2&lt;$J$4,$J$1,IF(D2&gt;$J$5,$J$2,(D2-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>70.677334127992609</v>
+      </c>
+      <c r="F2">
+        <f>IF(ABS($J$6-A2)&lt;5,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>275</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B26" si="0">(A3-$J$6)/$J$6</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C26" si="1">IF(B3&lt;0,-1*POWER(ABS(B3),(3-($J$3/4.5))),POWER(ABS(B3),(3-($J$3/4.5))))</f>
+        <v>-0.19842513149602492</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="2">($J$6*C3)+$J$6</f>
+        <v>440.86617767718633</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="3">IF(D3&lt;$J$4,$J$1,IF(D3&gt;$J$5,$J$2,(D3-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>81.118125512804198</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F26" si="4">IF(ABS($J$6-A3)&lt;5,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>-0.45454545454545453</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>-0.15885970244393161</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>462.62716365583765</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>90.366544553731003</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>325</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>-0.40909090909090912</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-0.12423565864449228</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>481.67038774552924</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>98.459914791849926</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>350</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>-0.36363636363636365</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-9.4382261884774651E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>498.08975596337393</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>105.43814628443393</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f>AVERAGE(J4,J5)</f>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>375</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>-0.31818181818181818</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>-6.9115561102646786E-2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>511.98644139354428</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>111.34423759225632</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>-0.27272727272727271</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>-4.8235486406878095E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>523.47048247621706</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>116.22495505239225</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>425</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>-0.22727272727272727</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-3.152175734685652E-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>532.66303345922893</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>120.13178922017228</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>450</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>-0.18181818181818182</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-1.8727812725378663E-2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>539.69970300104171</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>123.12237377544274</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>475</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>-0.13636363636363635</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>-9.571132733059505E-3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>544.7358769968173</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>125.26274772364737</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>500</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>-9.0909090909090912E-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>-3.7160687026661894E-3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>547.95616221353362</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>126.63136894075178</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>525</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>-4.5454545454545456E-2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>-7.3736142097480207E-4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>549.59445121846386</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>127.32764176784714</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>550</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>127.5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>575</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>7.3736142097480207E-4</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>550.40554878153614</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>127.67235823215286</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>600</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>3.7160687026661894E-3</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>552.04383778646638</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>128.36863105924823</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>625</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>9.571132733059505E-3</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>555.2641230031827</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>129.73725227635265</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>650</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>1.8727812725378663E-2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>560.30029699895829</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>131.87762622455728</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>675</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>3.152175734685652E-2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>567.33696654077107</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>134.86821077982771</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>700</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>4.8235486406878095E-2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>576.52951752378294</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>138.77504494760774</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>725</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>6.9115561102646786E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>588.01355860645572</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>143.65576240774368</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>750</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>9.4382261884774651E-2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>601.91024403662607</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>149.56185371556609</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>775</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.12423565864449228</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>618.3296122544707</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>156.54008520815006</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>800</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.15885970244393161</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>637.37283634416235</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>164.63345544626901</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>825</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.19842513149602492</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>659.13382232281367</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>173.88187448719583</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>850</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.24309161870377496</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>683.70039028707629</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>184.32266587200741</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <f>128*B2+128</f>
+        <v>58.181818181818187</v>
+      </c>
+      <c r="C29">
+        <f>128*C2+128</f>
+        <v>96.884272805916808</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:F44" si="5">128*D2+128</f>
+        <v>53414.350043254242</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="5"/>
+        <v>9174.6987683830539</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f>128*B3+128</f>
+        <v>64</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:F45" si="6">128*C3+128</f>
+        <v>102.60158316850881</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="5"/>
+        <v>56558.87074267985</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="5"/>
+        <v>10511.120065638937</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <f>128*B4+128</f>
+        <v>69.818181818181813</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="6"/>
+        <v>107.66595808717676</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="5"/>
+        <v>59344.276947947219</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="5"/>
+        <v>11694.917702877568</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <f>128*B5+128</f>
+        <v>75.636363636363626</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="6"/>
+        <v>112.09783569350499</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="5"/>
+        <v>61781.809631427743</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="5"/>
+        <v>12730.86909335679</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <f>128*B6+128</f>
+        <v>81.454545454545453</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="6"/>
+        <v>115.91907047874885</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>63883.488763311863</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="5"/>
+        <v>13624.082724407543</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <f>128*B7+128</f>
+        <v>87.27272727272728</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="6"/>
+        <v>119.15320817886121</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="5"/>
+        <v>65662.264498373668</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="5"/>
+        <v>14380.062411808809</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <f>128*B8+128</f>
+        <v>93.090909090909093</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="6"/>
+        <v>121.8258577399196</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="5"/>
+        <v>67132.221756955783</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="5"/>
+        <v>15004.794246706208</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <f>128*B9+128</f>
+        <v>98.909090909090907</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="6"/>
+        <v>123.96521505960237</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>68308.868282781303</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="5"/>
+        <v>15504.869020182052</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <f>128*B10+128</f>
+        <v>104.72727272727272</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="6"/>
+        <v>125.60283997115152</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="5"/>
+        <v>69209.561984133339</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="5"/>
+        <v>15887.663843256671</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <f>128*B11+128</f>
+        <v>110.54545454545455</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="6"/>
+        <v>126.77489501016838</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="5"/>
+        <v>69854.192255592614</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="5"/>
+        <v>16161.631708626863</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <f>128*B12+128</f>
+        <v>116.36363636363636</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="6"/>
+        <v>127.52434320605873</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="5"/>
+        <v>70266.388763332303</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="5"/>
+        <v>16336.815224416228</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <f>128*B13+128</f>
+        <v>122.18181818181819</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="6"/>
+        <v>127.90561773811523</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="5"/>
+        <v>70476.089755963374</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="5"/>
+        <v>16425.938146284432</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <f>128*B14+128</f>
+        <v>128</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="5"/>
+        <v>70528</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="5"/>
+        <v>16448</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <f>128*B15+128</f>
+        <v>133.81818181818181</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="6"/>
+        <v>128.09438226188476</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="5"/>
+        <v>70579.910244036626</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="5"/>
+        <v>16470.061853715568</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <f>128*B16+128</f>
+        <v>139.63636363636363</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="6"/>
+        <v>128.47565679394128</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="5"/>
+        <v>70789.611236667697</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="5"/>
+        <v>16559.184775583773</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <f>128*B17+128</f>
+        <v>145.45454545454544</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="6"/>
+        <v>129.22510498983161</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="5"/>
+        <v>71201.807744407386</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="5"/>
+        <v>16734.368291373139</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <f>128*B18+128</f>
+        <v>151.27272727272728</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="6"/>
+        <v>130.39716002884848</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="6"/>
+        <v>71846.438015866661</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="6"/>
+        <v>17008.336156743331</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <f>128*B19+128</f>
+        <v>157.09090909090909</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:F49" si="7">128*C19+128</f>
+        <v>132.03478494039763</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="7"/>
+        <v>72747.131717218697</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="7"/>
+        <v>17391.130979817946</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <f>128*B20+128</f>
+        <v>162.90909090909091</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="7"/>
+        <v>134.1741422600804</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="7"/>
+        <v>73923.778243044217</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="7"/>
+        <v>17891.205753293791</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <f>128*B21+128</f>
+        <v>168.72727272727272</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="7"/>
+        <v>136.84679182113879</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="7"/>
+        <v>75393.735501626332</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="7"/>
+        <v>18515.937588191191</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <f>128*B22+128</f>
+        <v>174.54545454545456</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="7"/>
+        <v>140.08092952125116</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="7"/>
+        <v>77172.511236688137</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="7"/>
+        <v>19271.917275592459</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>250</v>
+      </c>
+      <c r="C54">
+        <f>(B54-$J$6)/$J$6</f>
+        <v>-0.54545454545454541</v>
+      </c>
+      <c r="D54">
+        <f>IF(ABS($J$6-B54)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>275</v>
+      </c>
+      <c r="C55">
+        <f>(B55-$J$6)/$J$6</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D55">
+        <f>IF(ABS($J$6-B55)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>300</v>
+      </c>
+      <c r="C56">
+        <f>(B56-$J$6)/$J$6</f>
+        <v>-0.45454545454545453</v>
+      </c>
+      <c r="D56">
+        <f>IF(ABS($J$6-B56)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>325</v>
+      </c>
+      <c r="C57">
+        <f>(B57-$J$6)/$J$6</f>
+        <v>-0.40909090909090912</v>
+      </c>
+      <c r="D57">
+        <f>IF(ABS($J$6-B57)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>350</v>
+      </c>
+      <c r="C58">
+        <f>(B58-$J$6)/$J$6</f>
+        <v>-0.36363636363636365</v>
+      </c>
+      <c r="D58">
+        <f>IF(ABS($J$6-B58)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>375</v>
+      </c>
+      <c r="C59">
+        <f>(B59-$J$6)/$J$6</f>
+        <v>-0.31818181818181818</v>
+      </c>
+      <c r="D59">
+        <f>IF(ABS($J$6-B59)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>400</v>
+      </c>
+      <c r="N59">
+        <f>IF(M59&lt;$J$4,$J$1,IF(M59&gt;$J$5,$J$2,(M59-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>63.75</v>
+      </c>
+      <c r="O59">
+        <f>M59+($J$6-$J$7)</f>
+        <v>432</v>
+      </c>
+      <c r="P59">
+        <f>IF(O59&lt;$J$4,$J$1,IF(O59&gt;$J$5,$J$2,(O59-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>77.349999999999994</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>400</v>
+      </c>
+      <c r="C60">
+        <f>(B60-$J$6)/$J$6</f>
+        <v>-0.27272727272727271</v>
+      </c>
+      <c r="D60">
+        <f>IF(ABS($J$6-B60)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <v>500</v>
+      </c>
+      <c r="N60">
+        <f>IF(M60&lt;$J$4,$J$1,IF(M60&gt;$J$5,$J$2,(M60-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>106.25</v>
+      </c>
+      <c r="O60">
+        <f>M60+($J$6-$J$7)</f>
+        <v>532</v>
+      </c>
+      <c r="P60">
+        <f>IF(O60&lt;$J$4,$J$1,IF(O60&gt;$J$5,$J$2,(O60-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>119.85</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>425</v>
+      </c>
+      <c r="C61">
+        <f>(B61-$J$6)/$J$6</f>
+        <v>-0.22727272727272727</v>
+      </c>
+      <c r="D61">
+        <f>IF(ABS($J$6-B61)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>600</v>
+      </c>
+      <c r="N61">
+        <f>IF(M61&lt;$J$4,$J$1,IF(M61&gt;$J$5,$J$2,(M61-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>148.75</v>
+      </c>
+      <c r="O61">
+        <f>M61+($J$6-$J$7)</f>
+        <v>632</v>
+      </c>
+      <c r="P61">
+        <f>IF(O61&lt;$J$4,$J$1,IF(O61&gt;$J$5,$J$2,(O61-$J$4)*($J$2-$J$1)/($J$5-$J$4)+$J$1))</f>
+        <v>162.35</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>450</v>
+      </c>
+      <c r="C62">
+        <f>(B62-$J$6)/$J$6</f>
+        <v>-0.18181818181818182</v>
+      </c>
+      <c r="D62">
+        <f>IF(ABS($J$6-B62)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>475</v>
+      </c>
+      <c r="C63">
+        <f>(B63-$J$6)/$J$6</f>
+        <v>-0.13636363636363635</v>
+      </c>
+      <c r="D63">
+        <f>IF(ABS($J$6-B63)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>500</v>
+      </c>
+      <c r="C64">
+        <f>(B64-$J$6)/$J$6</f>
+        <v>-9.0909090909090912E-2</v>
+      </c>
+      <c r="D64">
+        <f>IF(ABS($J$6-B64)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>525</v>
+      </c>
+      <c r="C65">
+        <f>(B65-$J$6)/$J$6</f>
+        <v>-4.5454545454545456E-2</v>
+      </c>
+      <c r="D65">
+        <f>IF(ABS($J$6-B65)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>550</v>
+      </c>
+      <c r="C66">
+        <f>(B66-$J$6)/$J$6</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f>IF(ABS($J$6-B66)&lt;10,0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>575</v>
+      </c>
+      <c r="C67">
+        <f>(B67-$J$6)/$J$6</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="D67">
+        <f>IF(ABS($J$6-B67)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>600</v>
+      </c>
+      <c r="C68">
+        <f>(B68-$J$6)/$J$6</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="D68">
+        <f>IF(ABS($J$6-B68)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>625</v>
+      </c>
+      <c r="C69">
+        <f>(B69-$J$6)/$J$6</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="D69">
+        <f>IF(ABS($J$6-B69)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>650</v>
+      </c>
+      <c r="C70">
+        <f>(B70-$J$6)/$J$6</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="D70">
+        <f>IF(ABS($J$6-B70)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>675</v>
+      </c>
+      <c r="C71">
+        <f>(B71-$J$6)/$J$6</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="D71">
+        <f>IF(ABS($J$6-B71)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>700</v>
+      </c>
+      <c r="C72">
+        <f>(B72-$J$6)/$J$6</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="D72">
+        <f>IF(ABS($J$6-B72)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>725</v>
+      </c>
+      <c r="C73">
+        <f>(B73-$J$6)/$J$6</f>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="D73">
+        <f>IF(ABS($J$6-B73)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>750</v>
+      </c>
+      <c r="C74">
+        <f>(B74-$J$6)/$J$6</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="D74">
+        <f>IF(ABS($J$6-B74)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>775</v>
+      </c>
+      <c r="C75">
+        <f>(B75-$J$6)/$J$6</f>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="D75">
+        <f>IF(ABS($J$6-B75)&lt;10,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>800</v>
+      </c>
+      <c r="C76">
+        <f>(B76-$J$6)/$J$6</f>
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>825</v>
+      </c>
+      <c r="C77">
+        <f>(B77-$J$6)/$J$6</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>850</v>
+      </c>
+      <c r="C78">
+        <f>(B78-$J$6)/$J$6</f>
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2547,4 +4747,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>